<commit_message>
Fixed the enable pin being used
</commit_message>
<xml_diff>
--- a/Electronics/Swarmbot IO Assignment.xlsx
+++ b/Electronics/Swarmbot IO Assignment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skippy/Documents/Projects/Swarmbot/Electrical/Swarmbot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skippy/Documents/Projects/Swarmbot/Electronics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB24D4B5-FCA9-414E-BECC-4F6C20AE8971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADAA33C-EDFB-4040-A377-15C5CE17A08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="17500" xr2:uid="{60A99227-D3FC-F448-A78E-FF7E643B1505}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="80">
   <si>
     <t>IO0</t>
   </si>
@@ -147,12 +147,6 @@
     <t>Line Sensor 4</t>
   </si>
   <si>
-    <t>Port Sensor</t>
-  </si>
-  <si>
-    <t>Starboard Sensor</t>
-  </si>
-  <si>
     <t>Bat I</t>
   </si>
   <si>
@@ -234,12 +228,6 @@
     <t>Line Sensor LED</t>
   </si>
   <si>
-    <t>Motor Sensor 1</t>
-  </si>
-  <si>
-    <t>Motor Sensor 2</t>
-  </si>
-  <si>
     <t>Digital out</t>
   </si>
   <si>
@@ -250,6 +238,42 @@
   </si>
   <si>
     <t>Digital out (PWM)</t>
+  </si>
+  <si>
+    <t>IR 1</t>
+  </si>
+  <si>
+    <t>IR 2</t>
+  </si>
+  <si>
+    <t>IR 4</t>
+  </si>
+  <si>
+    <t>IR 3</t>
+  </si>
+  <si>
+    <t>Top PCB Version</t>
+  </si>
+  <si>
+    <t>Bottom PCB Version</t>
+  </si>
+  <si>
+    <t>IR 5</t>
+  </si>
+  <si>
+    <t>IR LEDS</t>
+  </si>
+  <si>
+    <t>&lt;-</t>
+  </si>
+  <si>
+    <t>Right Motor Sensor</t>
+  </si>
+  <si>
+    <t>Line Sensor 5</t>
+  </si>
+  <si>
+    <t>Left Motor Sensor</t>
   </si>
 </sst>
 </file>
@@ -615,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9720321F-9119-EB4D-99C2-316818D77AF4}">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -626,7 +650,7 @@
     <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -634,57 +658,57 @@
         <v>26</v>
       </c>
       <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" t="s">
-        <v>51</v>
-      </c>
       <c r="G1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C5">
         <v>36</v>
@@ -693,18 +717,21 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="H5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6">
         <v>39</v>
@@ -713,13 +740,16 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="H6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -733,16 +763,16 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="H7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -756,16 +786,16 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="H8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -779,16 +809,16 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="H9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -802,16 +832,16 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="H10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -825,16 +855,16 @@
         <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -848,16 +878,16 @@
         <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="H12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -871,16 +901,13 @@
         <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="J13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -894,16 +921,16 @@
         <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G14" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="H14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -917,24 +944,24 @@
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="H15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -951,13 +978,13 @@
         <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G17" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="H17" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -965,16 +992,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18">
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G18" t="s">
-        <v>63</v>
+        <v>30</v>
+      </c>
+      <c r="H18" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -982,16 +1012,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C19">
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G19" t="s">
         <v>63</v>
+      </c>
+      <c r="H19" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -999,16 +1032,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C20">
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G20" t="s">
-        <v>63</v>
+        <v>29</v>
+      </c>
+      <c r="H20" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1016,16 +1052,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C21">
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G21" t="s">
-        <v>63</v>
+        <v>40</v>
+      </c>
+      <c r="H21" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1033,16 +1072,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C22">
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G22" t="s">
-        <v>63</v>
+        <v>31</v>
+      </c>
+      <c r="H22" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1050,16 +1092,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C23">
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G23" t="s">
-        <v>63</v>
+        <v>36</v>
+      </c>
+      <c r="H23" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1076,13 +1121,13 @@
         <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1099,13 +1144,13 @@
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G25" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H25" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1122,10 +1167,10 @@
         <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1142,13 +1187,13 @@
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G27" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="H27" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1162,13 +1207,13 @@
         <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H28" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1182,13 +1227,13 @@
         <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G29" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="H29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1202,13 +1247,13 @@
         <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G30" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="H30" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1222,13 +1267,13 @@
         <v>18</v>
       </c>
       <c r="E31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G31" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1242,13 +1287,13 @@
         <v>19</v>
       </c>
       <c r="E32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G32" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1256,13 +1301,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
-      </c>
-      <c r="E33" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="G33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1276,13 +1318,13 @@
         <v>21</v>
       </c>
       <c r="E34" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G34" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="H34" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1290,13 +1332,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C35">
         <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G35" t="s">
         <v>23</v>
@@ -1307,13 +1349,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G36" t="s">
         <v>22</v>
@@ -1330,13 +1372,13 @@
         <v>22</v>
       </c>
       <c r="E37" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G37" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="H37" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1350,13 +1392,13 @@
         <v>23</v>
       </c>
       <c r="E38" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G38" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1364,10 +1406,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Cleaning up the stupid error with the pinout
</commit_message>
<xml_diff>
--- a/Electronics/Swarmbot IO Assignment.xlsx
+++ b/Electronics/Swarmbot IO Assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skippy/Documents/Projects/Swarmbot/Electronics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADAA33C-EDFB-4040-A377-15C5CE17A08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12E0979-F6D2-6645-A0BC-D32B20A7E4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="17500" xr2:uid="{60A99227-D3FC-F448-A78E-FF7E643B1505}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="79">
   <si>
     <t>IO0</t>
   </si>
@@ -262,9 +262,6 @@
   </si>
   <si>
     <t>IR LEDS</t>
-  </si>
-  <si>
-    <t>&lt;-</t>
   </si>
   <si>
     <t>Right Motor Sensor</t>
@@ -302,12 +299,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -322,9 +325,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,18 +643,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9720321F-9119-EB4D-99C2-316818D77AF4}">
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="99" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -670,40 +675,55 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G3" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G4" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -726,7 +746,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -749,7 +769,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -772,7 +792,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -795,7 +815,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -818,7 +838,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -835,13 +855,13 @@
         <v>50</v>
       </c>
       <c r="G10" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -858,13 +878,13 @@
         <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -881,13 +901,13 @@
         <v>50</v>
       </c>
       <c r="G12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -903,11 +923,14 @@
       <c r="E13" t="s">
         <v>50</v>
       </c>
-      <c r="J13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -927,10 +950,10 @@
         <v>77</v>
       </c>
       <c r="H14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -947,22 +970,27 @@
         <v>50</v>
       </c>
       <c r="G15" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="H15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G16" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -981,9 +1009,9 @@
         <v>50</v>
       </c>
       <c r="G17" t="s">
-        <v>78</v>
-      </c>
-      <c r="H17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1001,7 +1029,7 @@
         <v>50</v>
       </c>
       <c r="G18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H18" t="s">
         <v>67</v>
@@ -1021,10 +1049,10 @@
         <v>50</v>
       </c>
       <c r="G19" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="H19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1041,7 +1069,7 @@
         <v>50</v>
       </c>
       <c r="G20" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H20" t="s">
         <v>67</v>
@@ -1061,10 +1089,10 @@
         <v>50</v>
       </c>
       <c r="G21" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="H21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1081,10 +1109,10 @@
         <v>50</v>
       </c>
       <c r="G22" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="H22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1101,10 +1129,10 @@
         <v>50</v>
       </c>
       <c r="G23" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="H23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1124,10 +1152,10 @@
         <v>50</v>
       </c>
       <c r="G24" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1147,31 +1175,33 @@
         <v>50</v>
       </c>
       <c r="G25" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="H25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>0</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <v>11</v>
       </c>
-      <c r="E26" t="s">
-        <v>50</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="E26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -1190,7 +1220,7 @@
         <v>50</v>
       </c>
       <c r="G27" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="H27" t="s">
         <v>64</v>
@@ -1210,10 +1240,10 @@
         <v>50</v>
       </c>
       <c r="G28" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1230,10 +1260,10 @@
         <v>50</v>
       </c>
       <c r="G29" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="H29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1250,10 +1280,10 @@
         <v>50</v>
       </c>
       <c r="G30" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="H30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1270,10 +1300,10 @@
         <v>50</v>
       </c>
       <c r="G31" t="s">
-        <v>41</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
+      </c>
+      <c r="H31" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1290,22 +1320,27 @@
         <v>50</v>
       </c>
       <c r="G32" t="s">
-        <v>33</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>66</v>
+        <v>27</v>
+      </c>
+      <c r="H32" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G33" t="s">
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
@@ -1321,45 +1356,51 @@
         <v>50</v>
       </c>
       <c r="G34" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="H34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="2">
         <v>3</v>
       </c>
-      <c r="E35" t="s">
-        <v>50</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="2">
         <v>1</v>
       </c>
-      <c r="E36" t="s">
-        <v>50</v>
-      </c>
-      <c r="G36" t="s">
+      <c r="D36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
@@ -1375,7 +1416,7 @@
         <v>50</v>
       </c>
       <c r="G37" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H37" t="s">
         <v>65</v>
@@ -1394,23 +1435,22 @@
       <c r="E38" t="s">
         <v>50</v>
       </c>
-      <c r="G38" t="s">
-        <v>72</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="A39" s="2">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G39" t="s">
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="H39" s="2"/>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B73" s="1"/>

</xml_diff>